<commit_message>
Support other reason wording and template changes
</commit_message>
<xml_diff>
--- a/tet/templates/thesis_embargo_committee.xlsx
+++ b/tet/templates/thesis_embargo_committee.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmorrell/Documents/thesis_embargo_tools/tet/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC09A04A-C847-6A40-9543-3A8BF4DD7F6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C52F537-5745-264C-B4BB-84A59365DDFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,6 +32,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>For patent-related purposes only.</t>
         </r>
@@ -51,6 +52,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>A doctoral candidate is requesting a full embargo or an extension to the six-month embargo period which requires approval from the University Librarian, the Division Chair, the Vice Provost, and the Dean of Graduate Studies.</t>
     </r>
@@ -153,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -164,31 +166,43 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -972,7 +986,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4:C4"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1162,7 +1176,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="5" t="s">
         <v>13</v>

</xml_diff>